<commit_message>
origins and spell fix
</commit_message>
<xml_diff>
--- a/INFO H.xlsx
+++ b/INFO H.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kelvin\Documents\GitHub\Craft-to-Exile-Harmony-Server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDEF35FA-677E-4CC7-90AD-6399B1C8CE11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB6FE80C-0D30-4597-B5C1-01B6FA5CF9D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-22305" yWindow="3750" windowWidth="20430" windowHeight="12390" xr2:uid="{9AC52566-6148-4199-B6AD-F6619CE8FF62}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1233" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1258" uniqueCount="501">
   <si>
     <t>Mod Name</t>
   </si>
@@ -1526,6 +1526,30 @@
   </si>
   <si>
     <t>Less Greedy Piglins</t>
+  </si>
+  <si>
+    <t>Better Weather</t>
+  </si>
+  <si>
+    <t>Dungeons of Exile</t>
+  </si>
+  <si>
+    <t>Get Off My Lawn</t>
+  </si>
+  <si>
+    <t>Wild World</t>
+  </si>
+  <si>
+    <t>Common Expansion: Foodstuffs</t>
+  </si>
+  <si>
+    <t>Pet Owner</t>
+  </si>
+  <si>
+    <t>Respawnable Pets</t>
+  </si>
+  <si>
+    <t>Project: Save the Pets!</t>
   </si>
 </sst>
 </file>
@@ -2918,10 +2942,10 @@
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>
-  <dimension ref="A1:F98"/>
+  <dimension ref="A1:F106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4286,7 +4310,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>490</v>
       </c>
@@ -4297,7 +4321,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>492</v>
       </c>
@@ -4305,6 +4329,97 @@
         <v>73</v>
       </c>
       <c r="C98" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>493</v>
+      </c>
+      <c r="B99" t="s">
+        <v>73</v>
+      </c>
+      <c r="C99" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>494</v>
+      </c>
+      <c r="B100" t="s">
+        <v>73</v>
+      </c>
+      <c r="C100" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>495</v>
+      </c>
+      <c r="B101" t="s">
+        <v>73</v>
+      </c>
+      <c r="C101" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>496</v>
+      </c>
+      <c r="B102" t="s">
+        <v>73</v>
+      </c>
+      <c r="C102" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>497</v>
+      </c>
+      <c r="B103" t="s">
+        <v>73</v>
+      </c>
+      <c r="C103" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>498</v>
+      </c>
+      <c r="B104" t="s">
+        <v>73</v>
+      </c>
+      <c r="C104" t="s">
+        <v>73</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>499</v>
+      </c>
+      <c r="B105" t="s">
+        <v>73</v>
+      </c>
+      <c r="C105" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>500</v>
+      </c>
+      <c r="B106" t="s">
+        <v>73</v>
+      </c>
+      <c r="C106" t="s">
         <v>73</v>
       </c>
     </row>
@@ -4314,7 +4429,7 @@
       <sortCondition ref="D1"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="A2:A83 A85:A98">
+  <conditionalFormatting sqref="A2:A83 A85:A106">
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>C2="?"</formula>
     </cfRule>

</xml_diff>

<commit_message>
mod udpates and chjanges to gear
</commit_message>
<xml_diff>
--- a/INFO H.xlsx
+++ b/INFO H.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kelvin\Documents\GitHub\Craft-to-Exile-Harmony-Server\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kelvin Vuu\Documents\GitHub\Craft-to-Exile-Harmony-Server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1889A0E3-77A0-4A15-8955-9B5BE4D9574B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE064DF9-F869-4756-B804-A9357EE4AEDC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="2715" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="5" xr2:uid="{9AC52566-6148-4199-B6AD-F6619CE8FF62}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="4" xr2:uid="{9AC52566-6148-4199-B6AD-F6619CE8FF62}"/>
   </bookViews>
   <sheets>
     <sheet name="Mod List" sheetId="1" r:id="rId1"/>
@@ -28,6 +28,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Mod List'!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Runes!$A$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Runewords!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Uniques!$A$1:$V$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1821" uniqueCount="875">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1893" uniqueCount="932">
   <si>
     <t>Mod Name</t>
   </si>
@@ -2672,6 +2673,177 @@
   </si>
   <si>
     <t>Static</t>
+  </si>
+  <si>
+    <t>cloth_chest4</t>
+  </si>
+  <si>
+    <t>ormus_robes * 9</t>
+  </si>
+  <si>
+    <t>gorebreaker</t>
+  </si>
+  <si>
+    <t>frostbreath</t>
+  </si>
+  <si>
+    <t>mjolner</t>
+  </si>
+  <si>
+    <t>warbreaker</t>
+  </si>
+  <si>
+    <t>iron_hammer</t>
+  </si>
+  <si>
+    <t>diamond_hammer</t>
+  </si>
+  <si>
+    <t>aeternium_hammer</t>
+  </si>
+  <si>
+    <t>the_step</t>
+  </si>
+  <si>
+    <t>leather_boots4</t>
+  </si>
+  <si>
+    <t>plaguewalker</t>
+  </si>
+  <si>
+    <t>leather_boots3</t>
+  </si>
+  <si>
+    <t>sunspite</t>
+  </si>
+  <si>
+    <t>leather_boots2</t>
+  </si>
+  <si>
+    <t>snakeskin</t>
+  </si>
+  <si>
+    <t>dragons_talon</t>
+  </si>
+  <si>
+    <t>dusktoe</t>
+  </si>
+  <si>
+    <t>holy_march</t>
+  </si>
+  <si>
+    <t>cloth_boots3</t>
+  </si>
+  <si>
+    <t>crystal_shroud</t>
+  </si>
+  <si>
+    <t>cloth_boots4</t>
+  </si>
+  <si>
+    <t>ghast_wind</t>
+  </si>
+  <si>
+    <t>sparkoak</t>
+  </si>
+  <si>
+    <t>plate_boots2</t>
+  </si>
+  <si>
+    <t>root</t>
+  </si>
+  <si>
+    <t>plate_boots4</t>
+  </si>
+  <si>
+    <t>windshriek</t>
+  </si>
+  <si>
+    <t>the_iron_fortress</t>
+  </si>
+  <si>
+    <t>greeds_embrace</t>
+  </si>
+  <si>
+    <t>plate_chest3</t>
+  </si>
+  <si>
+    <t>hyrris_ire</t>
+  </si>
+  <si>
+    <t>leather_chest3</t>
+  </si>
+  <si>
+    <t>perfect_form_bow</t>
+  </si>
+  <si>
+    <t>perfect_form_xbow</t>
+  </si>
+  <si>
+    <t>the_covenant</t>
+  </si>
+  <si>
+    <t>cloth_chest3</t>
+  </si>
+  <si>
+    <t>shavronnes_wrappings</t>
+  </si>
+  <si>
+    <t>icetomb</t>
+  </si>
+  <si>
+    <t>plate_chest2</t>
+  </si>
+  <si>
+    <t>alphas_roar</t>
+  </si>
+  <si>
+    <t>leather_helmet4</t>
+  </si>
+  <si>
+    <t>the_visage</t>
+  </si>
+  <si>
+    <t>starkonjas_head</t>
+  </si>
+  <si>
+    <t>leather_helmet3</t>
+  </si>
+  <si>
+    <t>rime_gaze</t>
+  </si>
+  <si>
+    <t>griffons_eye</t>
+  </si>
+  <si>
+    <t>kiras_guardian</t>
+  </si>
+  <si>
+    <t>crown_of_ages</t>
+  </si>
+  <si>
+    <t>vampire_gaze</t>
+  </si>
+  <si>
+    <t>abyssus</t>
+  </si>
+  <si>
+    <t>hrimnors_resolve</t>
+  </si>
+  <si>
+    <t>plate_helmet3</t>
+  </si>
+  <si>
+    <t>plate_helmet4</t>
+  </si>
+  <si>
+    <t>plate_helmet2</t>
+  </si>
+  <si>
+    <t>cloth_helmet2</t>
+  </si>
+  <si>
+    <t>harlequin_crest</t>
   </si>
 </sst>
 </file>
@@ -7080,10 +7252,10 @@
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:V54"/>
+  <dimension ref="A1:V90"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B91" sqref="B91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7169,302 +7341,218 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>308</v>
+        <v>879</v>
       </c>
       <c r="B2" t="s">
-        <v>309</v>
-      </c>
-      <c r="C2" t="s">
-        <v>162</v>
-      </c>
-      <c r="D2" t="s">
-        <v>310</v>
-      </c>
-      <c r="E2" t="s">
-        <v>181</v>
-      </c>
-      <c r="F2" t="s">
-        <v>311</v>
-      </c>
-      <c r="G2" t="s">
-        <v>165</v>
-      </c>
-      <c r="H2" t="s">
-        <v>312</v>
-      </c>
-      <c r="I2" t="s">
-        <v>151</v>
-      </c>
-      <c r="J2" t="s">
-        <v>313</v>
+        <v>883</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>314</v>
+        <v>880</v>
       </c>
       <c r="B3" t="s">
-        <v>315</v>
-      </c>
-      <c r="C3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D3" t="s">
-        <v>316</v>
-      </c>
-      <c r="E3" t="s">
-        <v>158</v>
-      </c>
-      <c r="F3" t="s">
-        <v>317</v>
-      </c>
-      <c r="G3" t="s">
-        <v>200</v>
-      </c>
-      <c r="H3" t="s">
-        <v>318</v>
-      </c>
-      <c r="I3" t="s">
-        <v>137</v>
-      </c>
-      <c r="J3" t="s">
-        <v>318</v>
+        <v>883</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
       <c r="B4" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
       <c r="C4" t="s">
-        <v>204</v>
+        <v>162</v>
       </c>
       <c r="D4" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
       <c r="E4" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="F4" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
       <c r="G4" t="s">
-        <v>190</v>
+        <v>165</v>
       </c>
       <c r="H4" t="s">
-        <v>323</v>
+        <v>312</v>
+      </c>
+      <c r="I4" t="s">
+        <v>151</v>
+      </c>
+      <c r="J4" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
       <c r="B5" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
       <c r="C5" t="s">
-        <v>138</v>
+        <v>90</v>
       </c>
       <c r="D5" t="s">
-        <v>326</v>
+        <v>316</v>
       </c>
       <c r="E5" t="s">
-        <v>118</v>
+        <v>158</v>
       </c>
       <c r="F5" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
       <c r="G5" t="s">
-        <v>144</v>
+        <v>200</v>
       </c>
       <c r="H5" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
       <c r="I5" t="s">
-        <v>107</v>
+        <v>137</v>
       </c>
       <c r="J5" t="s">
-        <v>329</v>
-      </c>
-      <c r="K5" t="s">
-        <v>190</v>
-      </c>
-      <c r="L5" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
       <c r="B6" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
       <c r="C6" t="s">
-        <v>121</v>
+        <v>204</v>
       </c>
       <c r="D6" t="s">
-        <v>332</v>
+        <v>321</v>
       </c>
       <c r="E6" t="s">
-        <v>155</v>
+        <v>189</v>
       </c>
       <c r="F6" t="s">
         <v>322</v>
       </c>
       <c r="G6" t="s">
-        <v>166</v>
+        <v>190</v>
       </c>
       <c r="H6" t="s">
-        <v>333</v>
-      </c>
-      <c r="I6" t="s">
-        <v>183</v>
-      </c>
-      <c r="J6" t="s">
-        <v>311</v>
-      </c>
-      <c r="K6" t="s">
-        <v>151</v>
-      </c>
-      <c r="L6" t="s">
-        <v>334</v>
+        <v>323</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>335</v>
+        <v>858</v>
       </c>
       <c r="B7" t="s">
-        <v>336</v>
-      </c>
-      <c r="C7" t="s">
-        <v>155</v>
-      </c>
-      <c r="D7" t="s">
-        <v>337</v>
-      </c>
-      <c r="E7" t="s">
-        <v>160</v>
-      </c>
-      <c r="F7" t="s">
-        <v>338</v>
-      </c>
-      <c r="G7" t="s">
-        <v>132</v>
-      </c>
-      <c r="H7" t="s">
-        <v>339</v>
-      </c>
-      <c r="I7" t="s">
-        <v>151</v>
-      </c>
-      <c r="J7" t="s">
-        <v>334</v>
+        <v>859</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>340</v>
+        <v>324</v>
       </c>
       <c r="B8" t="s">
-        <v>341</v>
+        <v>325</v>
       </c>
       <c r="C8" t="s">
-        <v>123</v>
+        <v>138</v>
       </c>
       <c r="D8" t="s">
-        <v>317</v>
+        <v>326</v>
       </c>
       <c r="E8" t="s">
-        <v>155</v>
+        <v>118</v>
       </c>
       <c r="F8" t="s">
-        <v>317</v>
+        <v>327</v>
       </c>
       <c r="G8" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H8" t="s">
-        <v>342</v>
+        <v>328</v>
       </c>
       <c r="I8" t="s">
-        <v>160</v>
+        <v>107</v>
       </c>
       <c r="J8" t="s">
-        <v>342</v>
+        <v>329</v>
       </c>
       <c r="K8" t="s">
-        <v>132</v>
+        <v>190</v>
       </c>
       <c r="L8" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>343</v>
+        <v>330</v>
       </c>
       <c r="B9" t="s">
-        <v>344</v>
+        <v>331</v>
       </c>
       <c r="C9" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="D9" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="E9" t="s">
-        <v>107</v>
+        <v>155</v>
       </c>
       <c r="F9" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="G9" t="s">
-        <v>109</v>
+        <v>166</v>
       </c>
       <c r="H9" t="s">
-        <v>345</v>
+        <v>333</v>
       </c>
       <c r="I9" t="s">
-        <v>113</v>
+        <v>183</v>
       </c>
       <c r="J9" t="s">
-        <v>346</v>
+        <v>311</v>
       </c>
       <c r="K9" t="s">
         <v>151</v>
       </c>
       <c r="L9" t="s">
-        <v>313</v>
+        <v>334</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>347</v>
+        <v>335</v>
       </c>
       <c r="B10" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
       <c r="C10" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="D10" t="s">
+        <v>337</v>
+      </c>
+      <c r="E10" t="s">
+        <v>160</v>
+      </c>
+      <c r="F10" t="s">
+        <v>338</v>
+      </c>
+      <c r="G10" t="s">
+        <v>132</v>
+      </c>
+      <c r="H10" t="s">
         <v>339</v>
-      </c>
-      <c r="E10" t="s">
-        <v>149</v>
-      </c>
-      <c r="F10" t="s">
-        <v>349</v>
-      </c>
-      <c r="G10" t="s">
-        <v>137</v>
-      </c>
-      <c r="H10" t="s">
-        <v>350</v>
       </c>
       <c r="I10" t="s">
         <v>151</v>
@@ -7475,322 +7563,172 @@
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>351</v>
+        <v>893</v>
       </c>
       <c r="B11" t="s">
-        <v>352</v>
-      </c>
-      <c r="C11" t="s">
-        <v>155</v>
-      </c>
-      <c r="D11" t="s">
-        <v>310</v>
-      </c>
-      <c r="E11" t="s">
-        <v>154</v>
-      </c>
-      <c r="F11" t="s">
-        <v>353</v>
-      </c>
-      <c r="G11" t="s">
-        <v>151</v>
-      </c>
-      <c r="H11" t="s">
-        <v>334</v>
+        <v>894</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>354</v>
+        <v>895</v>
       </c>
       <c r="B12" t="s">
-        <v>355</v>
-      </c>
-      <c r="C12" t="s">
-        <v>155</v>
-      </c>
-      <c r="D12" t="s">
-        <v>329</v>
-      </c>
-      <c r="E12" t="s">
-        <v>154</v>
-      </c>
-      <c r="F12" t="s">
-        <v>356</v>
-      </c>
-      <c r="G12" t="s">
-        <v>132</v>
-      </c>
-      <c r="H12" t="s">
-        <v>356</v>
+        <v>896</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>357</v>
+        <v>897</v>
       </c>
       <c r="B13" t="s">
-        <v>358</v>
-      </c>
-      <c r="C13" t="s">
-        <v>155</v>
-      </c>
-      <c r="D13" t="s">
-        <v>338</v>
-      </c>
-      <c r="E13" t="s">
-        <v>155</v>
-      </c>
-      <c r="F13" t="s">
-        <v>339</v>
-      </c>
-      <c r="G13" t="s">
-        <v>103</v>
-      </c>
-      <c r="H13" t="s">
-        <v>345</v>
-      </c>
-      <c r="I13" t="s">
-        <v>154</v>
-      </c>
-      <c r="J13" t="s">
-        <v>359</v>
-      </c>
-      <c r="K13" t="s">
-        <v>151</v>
-      </c>
-      <c r="L13" t="s">
-        <v>334</v>
+        <v>896</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>360</v>
+        <v>340</v>
       </c>
       <c r="B14" t="s">
-        <v>361</v>
+        <v>341</v>
       </c>
       <c r="C14" t="s">
+        <v>123</v>
+      </c>
+      <c r="D14" t="s">
+        <v>317</v>
+      </c>
+      <c r="E14" t="s">
         <v>155</v>
       </c>
-      <c r="D14" t="s">
-        <v>353</v>
-      </c>
-      <c r="E14" t="s">
-        <v>184</v>
-      </c>
       <c r="F14" t="s">
-        <v>362</v>
+        <v>317</v>
       </c>
       <c r="G14" t="s">
         <v>143</v>
       </c>
       <c r="H14" t="s">
-        <v>363</v>
+        <v>342</v>
       </c>
       <c r="I14" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="J14" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="K14" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="L14" t="s">
-        <v>364</v>
+        <v>322</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>365</v>
+        <v>343</v>
       </c>
       <c r="B15" t="s">
-        <v>366</v>
+        <v>344</v>
       </c>
       <c r="C15" t="s">
-        <v>103</v>
+        <v>137</v>
       </c>
       <c r="D15" t="s">
+        <v>337</v>
+      </c>
+      <c r="E15" t="s">
+        <v>107</v>
+      </c>
+      <c r="F15" t="s">
+        <v>329</v>
+      </c>
+      <c r="G15" t="s">
+        <v>109</v>
+      </c>
+      <c r="H15" t="s">
         <v>345</v>
       </c>
-      <c r="E15" t="s">
-        <v>134</v>
-      </c>
-      <c r="F15" t="s">
-        <v>367</v>
-      </c>
-      <c r="G15" t="s">
-        <v>155</v>
-      </c>
-      <c r="H15" t="s">
-        <v>337</v>
-      </c>
       <c r="I15" t="s">
-        <v>167</v>
+        <v>113</v>
       </c>
       <c r="J15" t="s">
-        <v>359</v>
+        <v>346</v>
       </c>
       <c r="K15" t="s">
         <v>151</v>
       </c>
       <c r="L15" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>368</v>
+        <v>910</v>
       </c>
       <c r="B16" t="s">
-        <v>369</v>
-      </c>
-      <c r="C16" t="s">
-        <v>118</v>
-      </c>
-      <c r="D16" t="s">
-        <v>370</v>
-      </c>
-      <c r="E16" t="s">
-        <v>117</v>
-      </c>
-      <c r="F16" t="s">
-        <v>370</v>
-      </c>
-      <c r="G16" t="s">
-        <v>154</v>
-      </c>
-      <c r="H16" t="s">
-        <v>370</v>
-      </c>
-      <c r="I16" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>876</v>
+      </c>
+      <c r="B17" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>912</v>
+      </c>
+      <c r="B18" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>347</v>
+      </c>
+      <c r="B19" t="s">
+        <v>348</v>
+      </c>
+      <c r="C19" t="s">
+        <v>167</v>
+      </c>
+      <c r="D19" t="s">
+        <v>339</v>
+      </c>
+      <c r="E19" t="s">
         <v>149</v>
       </c>
-      <c r="J16" t="s">
-        <v>370</v>
-      </c>
-      <c r="K16" t="s">
+      <c r="F19" t="s">
+        <v>349</v>
+      </c>
+      <c r="G19" t="s">
+        <v>137</v>
+      </c>
+      <c r="H19" t="s">
+        <v>350</v>
+      </c>
+      <c r="I19" t="s">
         <v>151</v>
       </c>
-      <c r="L16" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>372</v>
-      </c>
-      <c r="B17" t="s">
-        <v>373</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="J19" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>351</v>
+      </c>
+      <c r="B20" t="s">
+        <v>352</v>
+      </c>
+      <c r="C20" t="s">
         <v>155</v>
       </c>
-      <c r="D17" t="s">
-        <v>374</v>
-      </c>
-      <c r="E17" t="s">
-        <v>155</v>
-      </c>
-      <c r="F17" t="s">
-        <v>375</v>
-      </c>
-      <c r="G17" t="s">
-        <v>166</v>
-      </c>
-      <c r="H17" t="s">
-        <v>376</v>
-      </c>
-      <c r="I17" t="s">
-        <v>157</v>
-      </c>
-      <c r="J17" t="s">
-        <v>376</v>
-      </c>
-      <c r="K17" t="s">
-        <v>143</v>
-      </c>
-      <c r="L17" t="s">
-        <v>377</v>
-      </c>
-      <c r="M17" t="s">
-        <v>151</v>
-      </c>
-      <c r="N17" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>379</v>
-      </c>
-      <c r="B18" t="s">
-        <v>380</v>
-      </c>
-      <c r="C18" t="s">
-        <v>143</v>
-      </c>
-      <c r="D18" t="s">
-        <v>381</v>
-      </c>
-      <c r="E18" t="s">
-        <v>149</v>
-      </c>
-      <c r="F18" t="s">
-        <v>381</v>
-      </c>
-      <c r="G18" t="s">
-        <v>154</v>
-      </c>
-      <c r="H18" t="s">
-        <v>381</v>
-      </c>
-      <c r="I18" t="s">
-        <v>132</v>
-      </c>
-      <c r="J18" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>382</v>
-      </c>
-      <c r="B19" t="s">
-        <v>383</v>
-      </c>
-      <c r="C19" t="s">
-        <v>204</v>
-      </c>
-      <c r="D19" t="s">
-        <v>374</v>
-      </c>
-      <c r="E19" t="s">
-        <v>154</v>
-      </c>
-      <c r="F19" t="s">
-        <v>353</v>
-      </c>
-      <c r="G19" t="s">
-        <v>160</v>
-      </c>
-      <c r="H19" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>385</v>
-      </c>
-      <c r="B20" t="s">
-        <v>386</v>
-      </c>
-      <c r="C20" t="s">
-        <v>204</v>
-      </c>
       <c r="D20" t="s">
-        <v>374</v>
+        <v>310</v>
       </c>
       <c r="E20" t="s">
         <v>154</v>
@@ -7799,1125 +7737,1652 @@
         <v>353</v>
       </c>
       <c r="G20" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="H20" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>387</v>
+        <v>354</v>
       </c>
       <c r="B21" t="s">
-        <v>388</v>
+        <v>355</v>
       </c>
       <c r="C21" t="s">
-        <v>123</v>
+        <v>155</v>
       </c>
       <c r="D21" t="s">
-        <v>317</v>
+        <v>329</v>
       </c>
       <c r="E21" t="s">
-        <v>101</v>
+        <v>154</v>
       </c>
       <c r="F21" t="s">
-        <v>322</v>
+        <v>356</v>
       </c>
       <c r="G21" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="H21" t="s">
-        <v>389</v>
-      </c>
-      <c r="I21" t="s">
-        <v>143</v>
-      </c>
-      <c r="J21" t="s">
-        <v>390</v>
-      </c>
-      <c r="K21" t="s">
-        <v>122</v>
-      </c>
-      <c r="L21" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>391</v>
+        <v>357</v>
       </c>
       <c r="B22" t="s">
-        <v>392</v>
+        <v>358</v>
       </c>
       <c r="C22" t="s">
-        <v>123</v>
+        <v>155</v>
       </c>
       <c r="D22" t="s">
         <v>338</v>
       </c>
       <c r="E22" t="s">
-        <v>143</v>
+        <v>155</v>
       </c>
       <c r="F22" t="s">
-        <v>393</v>
+        <v>339</v>
       </c>
       <c r="G22" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="H22" t="s">
         <v>345</v>
       </c>
       <c r="I22" t="s">
+        <v>154</v>
+      </c>
+      <c r="J22" t="s">
+        <v>359</v>
+      </c>
+      <c r="K22" t="s">
+        <v>151</v>
+      </c>
+      <c r="L22" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>360</v>
+      </c>
+      <c r="B23" t="s">
+        <v>361</v>
+      </c>
+      <c r="C23" t="s">
+        <v>155</v>
+      </c>
+      <c r="D23" t="s">
+        <v>353</v>
+      </c>
+      <c r="E23" t="s">
+        <v>184</v>
+      </c>
+      <c r="F23" t="s">
+        <v>362</v>
+      </c>
+      <c r="G23" t="s">
+        <v>143</v>
+      </c>
+      <c r="H23" t="s">
+        <v>363</v>
+      </c>
+      <c r="I23" t="s">
         <v>150</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J23" t="s">
         <v>345</v>
       </c>
-      <c r="K22" t="s">
-        <v>122</v>
-      </c>
-      <c r="L22" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>394</v>
-      </c>
-      <c r="B23" t="s">
-        <v>395</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="K23" t="s">
+        <v>151</v>
+      </c>
+      <c r="L23" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>365</v>
+      </c>
+      <c r="B24" t="s">
+        <v>366</v>
+      </c>
+      <c r="C24" t="s">
         <v>103</v>
-      </c>
-      <c r="D23" t="s">
-        <v>345</v>
-      </c>
-      <c r="E23" t="s">
-        <v>123</v>
-      </c>
-      <c r="F23" t="s">
-        <v>396</v>
-      </c>
-      <c r="G23" t="s">
-        <v>200</v>
-      </c>
-      <c r="H23" t="s">
-        <v>397</v>
-      </c>
-      <c r="I23" t="s">
-        <v>121</v>
-      </c>
-      <c r="J23" t="s">
-        <v>390</v>
-      </c>
-      <c r="K23" t="s">
-        <v>122</v>
-      </c>
-      <c r="L23" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>398</v>
-      </c>
-      <c r="B24" t="s">
-        <v>399</v>
-      </c>
-      <c r="C24" t="s">
-        <v>109</v>
       </c>
       <c r="D24" t="s">
         <v>345</v>
       </c>
       <c r="E24" t="s">
+        <v>134</v>
+      </c>
+      <c r="F24" t="s">
+        <v>367</v>
+      </c>
+      <c r="G24" t="s">
+        <v>155</v>
+      </c>
+      <c r="H24" t="s">
+        <v>337</v>
+      </c>
+      <c r="I24" t="s">
+        <v>167</v>
+      </c>
+      <c r="J24" t="s">
+        <v>359</v>
+      </c>
+      <c r="K24" t="s">
+        <v>151</v>
+      </c>
+      <c r="L24" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>368</v>
+      </c>
+      <c r="B25" t="s">
+        <v>369</v>
+      </c>
+      <c r="C25" t="s">
+        <v>118</v>
+      </c>
+      <c r="D25" t="s">
+        <v>370</v>
+      </c>
+      <c r="E25" t="s">
+        <v>117</v>
+      </c>
+      <c r="F25" t="s">
+        <v>370</v>
+      </c>
+      <c r="G25" t="s">
+        <v>154</v>
+      </c>
+      <c r="H25" t="s">
+        <v>370</v>
+      </c>
+      <c r="I25" t="s">
+        <v>149</v>
+      </c>
+      <c r="J25" t="s">
+        <v>370</v>
+      </c>
+      <c r="K25" t="s">
+        <v>151</v>
+      </c>
+      <c r="L25" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>372</v>
+      </c>
+      <c r="B26" t="s">
+        <v>373</v>
+      </c>
+      <c r="C26" t="s">
+        <v>155</v>
+      </c>
+      <c r="D26" t="s">
+        <v>374</v>
+      </c>
+      <c r="E26" t="s">
+        <v>155</v>
+      </c>
+      <c r="F26" t="s">
+        <v>375</v>
+      </c>
+      <c r="G26" t="s">
+        <v>166</v>
+      </c>
+      <c r="H26" t="s">
+        <v>376</v>
+      </c>
+      <c r="I26" t="s">
+        <v>157</v>
+      </c>
+      <c r="J26" t="s">
+        <v>376</v>
+      </c>
+      <c r="K26" t="s">
+        <v>143</v>
+      </c>
+      <c r="L26" t="s">
+        <v>377</v>
+      </c>
+      <c r="M26" t="s">
+        <v>151</v>
+      </c>
+      <c r="N26" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>878</v>
+      </c>
+      <c r="B27" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>379</v>
+      </c>
+      <c r="B28" t="s">
+        <v>380</v>
+      </c>
+      <c r="C28" t="s">
+        <v>143</v>
+      </c>
+      <c r="D28" t="s">
+        <v>381</v>
+      </c>
+      <c r="E28" t="s">
+        <v>149</v>
+      </c>
+      <c r="F28" t="s">
+        <v>381</v>
+      </c>
+      <c r="G28" t="s">
+        <v>154</v>
+      </c>
+      <c r="H28" t="s">
+        <v>381</v>
+      </c>
+      <c r="I28" t="s">
+        <v>132</v>
+      </c>
+      <c r="J28" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>382</v>
+      </c>
+      <c r="B29" t="s">
+        <v>383</v>
+      </c>
+      <c r="C29" t="s">
+        <v>204</v>
+      </c>
+      <c r="D29" t="s">
+        <v>374</v>
+      </c>
+      <c r="E29" t="s">
+        <v>154</v>
+      </c>
+      <c r="F29" t="s">
+        <v>353</v>
+      </c>
+      <c r="G29" t="s">
+        <v>160</v>
+      </c>
+      <c r="H29" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>385</v>
+      </c>
+      <c r="B30" t="s">
+        <v>386</v>
+      </c>
+      <c r="C30" t="s">
+        <v>204</v>
+      </c>
+      <c r="D30" t="s">
+        <v>374</v>
+      </c>
+      <c r="E30" t="s">
+        <v>154</v>
+      </c>
+      <c r="F30" t="s">
+        <v>353</v>
+      </c>
+      <c r="G30" t="s">
+        <v>160</v>
+      </c>
+      <c r="H30" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>877</v>
+      </c>
+      <c r="B31" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>387</v>
+      </c>
+      <c r="B32" t="s">
+        <v>388</v>
+      </c>
+      <c r="C32" t="s">
         <v>123</v>
       </c>
-      <c r="F24" t="s">
+      <c r="D32" t="s">
+        <v>317</v>
+      </c>
+      <c r="E32" t="s">
+        <v>101</v>
+      </c>
+      <c r="F32" t="s">
+        <v>322</v>
+      </c>
+      <c r="G32" t="s">
+        <v>137</v>
+      </c>
+      <c r="H32" t="s">
+        <v>389</v>
+      </c>
+      <c r="I32" t="s">
+        <v>143</v>
+      </c>
+      <c r="J32" t="s">
+        <v>390</v>
+      </c>
+      <c r="K32" t="s">
+        <v>122</v>
+      </c>
+      <c r="L32" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>892</v>
+      </c>
+      <c r="B33" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>391</v>
+      </c>
+      <c r="B34" t="s">
+        <v>392</v>
+      </c>
+      <c r="C34" t="s">
+        <v>123</v>
+      </c>
+      <c r="D34" t="s">
+        <v>338</v>
+      </c>
+      <c r="E34" t="s">
+        <v>143</v>
+      </c>
+      <c r="F34" t="s">
+        <v>393</v>
+      </c>
+      <c r="G34" t="s">
+        <v>121</v>
+      </c>
+      <c r="H34" t="s">
+        <v>345</v>
+      </c>
+      <c r="I34" t="s">
+        <v>150</v>
+      </c>
+      <c r="J34" t="s">
+        <v>345</v>
+      </c>
+      <c r="K34" t="s">
+        <v>122</v>
+      </c>
+      <c r="L34" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>888</v>
+      </c>
+      <c r="B35" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>886</v>
+      </c>
+      <c r="B36" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>890</v>
+      </c>
+      <c r="B37" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>884</v>
+      </c>
+      <c r="B38" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>891</v>
+      </c>
+      <c r="B39" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>394</v>
+      </c>
+      <c r="B40" t="s">
+        <v>395</v>
+      </c>
+      <c r="C40" t="s">
+        <v>103</v>
+      </c>
+      <c r="D40" t="s">
+        <v>345</v>
+      </c>
+      <c r="E40" t="s">
+        <v>123</v>
+      </c>
+      <c r="F40" t="s">
+        <v>396</v>
+      </c>
+      <c r="G40" t="s">
+        <v>200</v>
+      </c>
+      <c r="H40" t="s">
+        <v>397</v>
+      </c>
+      <c r="I40" t="s">
+        <v>121</v>
+      </c>
+      <c r="J40" t="s">
+        <v>390</v>
+      </c>
+      <c r="K40" t="s">
+        <v>122</v>
+      </c>
+      <c r="L40" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>398</v>
+      </c>
+      <c r="B41" t="s">
+        <v>399</v>
+      </c>
+      <c r="C41" t="s">
+        <v>109</v>
+      </c>
+      <c r="D41" t="s">
+        <v>345</v>
+      </c>
+      <c r="E41" t="s">
+        <v>123</v>
+      </c>
+      <c r="F41" t="s">
         <v>400</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G41" t="s">
         <v>143</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H41" t="s">
         <v>350</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I41" t="s">
         <v>137</v>
       </c>
-      <c r="J24" t="s">
+      <c r="J41" t="s">
         <v>350</v>
       </c>
-      <c r="K24" t="s">
+      <c r="K41" t="s">
         <v>106</v>
       </c>
-      <c r="L24" t="s">
+      <c r="L41" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>906</v>
+      </c>
+      <c r="B42" t="s">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>401</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B43" t="s">
         <v>402</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C43" t="s">
         <v>123</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D43" t="s">
         <v>374</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E43" t="s">
         <v>123</v>
       </c>
-      <c r="F25" t="s">
+      <c r="F43" t="s">
         <v>403</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G43" t="s">
         <v>118</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H43" t="s">
         <v>404</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I43" t="s">
         <v>190</v>
       </c>
-      <c r="J25" t="s">
+      <c r="J43" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>908</v>
+      </c>
+      <c r="B44" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>909</v>
+      </c>
+      <c r="B45" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>405</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B46" t="s">
         <v>406</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C46" t="s">
         <v>167</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D46" t="s">
         <v>339</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E46" t="s">
         <v>149</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F46" t="s">
         <v>349</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G46" t="s">
         <v>137</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H46" t="s">
         <v>350</v>
       </c>
-      <c r="I26" t="s">
+      <c r="I46" t="s">
         <v>122</v>
       </c>
-      <c r="J26" t="s">
+      <c r="J46" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>407</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B47" t="s">
         <v>408</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C47" t="s">
         <v>123</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D47" t="s">
         <v>310</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E47" t="s">
         <v>154</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F47" t="s">
         <v>353</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G47" t="s">
         <v>122</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H47" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>409</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B48" t="s">
         <v>410</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C48" t="s">
         <v>123</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D48" t="s">
         <v>329</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E48" t="s">
         <v>154</v>
       </c>
-      <c r="F28" t="s">
+      <c r="F48" t="s">
         <v>356</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G48" t="s">
         <v>132</v>
       </c>
-      <c r="H28" t="s">
+      <c r="H48" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>357</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B49" t="s">
         <v>411</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C49" t="s">
         <v>123</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D49" t="s">
         <v>338</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E49" t="s">
         <v>123</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F49" t="s">
         <v>339</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G49" t="s">
         <v>103</v>
       </c>
-      <c r="H29" t="s">
+      <c r="H49" t="s">
         <v>345</v>
       </c>
-      <c r="I29" t="s">
+      <c r="I49" t="s">
         <v>154</v>
       </c>
-      <c r="J29" t="s">
+      <c r="J49" t="s">
         <v>359</v>
       </c>
-      <c r="K29" t="s">
+      <c r="K49" t="s">
         <v>122</v>
       </c>
-      <c r="L29" t="s">
+      <c r="L49" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>412</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B50" t="s">
         <v>413</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C50" t="s">
         <v>123</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D50" t="s">
         <v>337</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E50" t="s">
         <v>137</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F50" t="s">
         <v>414</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G50" t="s">
         <v>200</v>
       </c>
-      <c r="H30" t="s">
+      <c r="H50" t="s">
         <v>414</v>
       </c>
-      <c r="I30" t="s">
+      <c r="I50" t="s">
         <v>109</v>
       </c>
-      <c r="J30" t="s">
+      <c r="J50" t="s">
         <v>414</v>
       </c>
-      <c r="K30" t="s">
+      <c r="K50" t="s">
         <v>110</v>
       </c>
-      <c r="L30" t="s">
+      <c r="L50" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>415</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B51" t="s">
         <v>416</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C51" t="s">
         <v>123</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D51" t="s">
         <v>417</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E51" t="s">
         <v>200</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F51" t="s">
         <v>414</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G51" t="s">
         <v>108</v>
       </c>
-      <c r="H31" t="s">
+      <c r="H51" t="s">
         <v>418</v>
       </c>
-      <c r="I31" t="s">
+      <c r="I51" t="s">
         <v>134</v>
       </c>
-      <c r="J31" t="s">
+      <c r="J51" t="s">
         <v>418</v>
       </c>
-      <c r="K31" t="s">
+      <c r="K51" t="s">
         <v>148</v>
       </c>
-      <c r="L31" t="s">
+      <c r="L51" t="s">
         <v>362</v>
       </c>
-      <c r="M31" t="s">
+      <c r="M51" t="s">
         <v>151</v>
       </c>
-      <c r="N31" t="s">
+      <c r="N51" t="s">
         <v>419</v>
       </c>
-      <c r="O31" t="s">
+      <c r="O51" t="s">
         <v>122</v>
       </c>
-      <c r="P31" t="s">
+      <c r="P51" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>420</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B52" t="s">
         <v>421</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C52" t="s">
         <v>143</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D52" t="s">
         <v>422</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E52" t="s">
         <v>90</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F52" t="s">
         <v>423</v>
       </c>
-      <c r="G32" t="s">
+      <c r="G52" t="s">
         <v>144</v>
       </c>
-      <c r="H32" t="s">
+      <c r="H52" t="s">
         <v>424</v>
       </c>
-      <c r="I32" t="s">
+      <c r="I52" t="s">
         <v>190</v>
       </c>
-      <c r="J32" t="s">
+      <c r="J52" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>425</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B53" t="s">
         <v>426</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C53" t="s">
         <v>160</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D53" t="s">
         <v>322</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E53" t="s">
         <v>166</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F53" t="s">
         <v>427</v>
       </c>
-      <c r="G33" t="s">
+      <c r="G53" t="s">
         <v>151</v>
       </c>
-      <c r="H33" t="s">
+      <c r="H53" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>428</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B54" t="s">
         <v>429</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C54" t="s">
         <v>101</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D54" t="s">
         <v>337</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E54" t="s">
         <v>132</v>
       </c>
-      <c r="F34" t="s">
+      <c r="F54" t="s">
         <v>367</v>
       </c>
-      <c r="G34" t="s">
+      <c r="G54" t="s">
         <v>101</v>
       </c>
-      <c r="H34" t="s">
+      <c r="H54" t="s">
         <v>322</v>
       </c>
-      <c r="I34" t="s">
+      <c r="I54" t="s">
         <v>121</v>
       </c>
-      <c r="J34" t="s">
+      <c r="J54" t="s">
         <v>430</v>
       </c>
-      <c r="K34" t="s">
+      <c r="K54" t="s">
         <v>189</v>
       </c>
-      <c r="L34" t="s">
+      <c r="L54" t="s">
         <v>430</v>
       </c>
-      <c r="M34" t="s">
+      <c r="M54" t="s">
         <v>190</v>
       </c>
-      <c r="N34" t="s">
+      <c r="N54" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>431</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B55" t="s">
         <v>432</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C55" t="s">
         <v>194</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D55" t="s">
         <v>433</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E55" t="s">
         <v>112</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F55" t="s">
         <v>345</v>
       </c>
-      <c r="G35" t="s">
+      <c r="G55" t="s">
         <v>303</v>
       </c>
-      <c r="H35" t="s">
+      <c r="H55" t="s">
         <v>434</v>
       </c>
-      <c r="I35" t="s">
+      <c r="I55" t="s">
         <v>115</v>
       </c>
-      <c r="J35" t="s">
+      <c r="J55" t="s">
         <v>359</v>
       </c>
-      <c r="K35" t="s">
+      <c r="K55" t="s">
         <v>190</v>
       </c>
-      <c r="L35" t="s">
+      <c r="L55" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>898</v>
+      </c>
+      <c r="B56" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>900</v>
+      </c>
+      <c r="B57" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>902</v>
+      </c>
+      <c r="B58" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>435</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B59" t="s">
         <v>436</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C59" t="s">
         <v>189</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D59" t="s">
         <v>322</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E59" t="s">
         <v>101</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F59" t="s">
         <v>356</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G59" t="s">
         <v>158</v>
       </c>
-      <c r="H36" t="s">
+      <c r="H59" t="s">
         <v>353</v>
       </c>
-      <c r="I36" t="s">
+      <c r="I59" t="s">
         <v>174</v>
       </c>
-      <c r="J36" t="s">
+      <c r="J59" t="s">
         <v>437</v>
       </c>
-      <c r="K36" t="s">
+      <c r="K59" t="s">
         <v>190</v>
       </c>
-      <c r="L36" t="s">
+      <c r="L59" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>438</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B60" t="s">
         <v>439</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C60" t="s">
         <v>101</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D60" t="s">
         <v>321</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E60" t="s">
         <v>132</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F60" t="s">
         <v>440</v>
       </c>
-      <c r="G37" t="s">
+      <c r="G60" t="s">
         <v>204</v>
       </c>
-      <c r="H37" t="s">
+      <c r="H60" t="s">
         <v>350</v>
       </c>
-      <c r="I37" t="s">
+      <c r="I60" t="s">
         <v>190</v>
       </c>
-      <c r="J37" t="s">
+      <c r="J60" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>913</v>
+      </c>
+      <c r="B61" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>904</v>
+      </c>
+      <c r="B62" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>442</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B63" t="s">
         <v>443</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C63" t="s">
         <v>143</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D63" t="s">
         <v>374</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E63" t="s">
         <v>145</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F63" t="s">
         <v>311</v>
       </c>
-      <c r="G38" t="s">
+      <c r="G63" t="s">
         <v>147</v>
       </c>
-      <c r="H38" t="s">
+      <c r="H63" t="s">
         <v>311</v>
       </c>
-      <c r="I38" t="s">
+      <c r="I63" t="s">
         <v>149</v>
       </c>
-      <c r="J38" t="s">
+      <c r="J63" t="s">
         <v>444</v>
       </c>
-      <c r="K38" t="s">
+      <c r="K63" t="s">
         <v>190</v>
       </c>
-      <c r="L38" t="s">
+      <c r="L63" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>903</v>
+      </c>
+      <c r="B64" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>445</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B65" t="s">
         <v>446</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C65" t="s">
         <v>167</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D65" t="s">
         <v>339</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E65" t="s">
         <v>149</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F65" t="s">
         <v>349</v>
       </c>
-      <c r="G39" t="s">
+      <c r="G65" t="s">
         <v>137</v>
       </c>
-      <c r="H39" t="s">
+      <c r="H65" t="s">
         <v>350</v>
       </c>
-      <c r="I39" t="s">
+      <c r="I65" t="s">
         <v>190</v>
       </c>
-      <c r="J39" t="s">
+      <c r="J65" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>447</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B66" t="s">
         <v>448</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C66" t="s">
         <v>101</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D66" t="s">
         <v>310</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E66" t="s">
         <v>154</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F66" t="s">
         <v>353</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G66" t="s">
         <v>190</v>
       </c>
-      <c r="H40" t="s">
+      <c r="H66" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>449</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B67" t="s">
         <v>450</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C67" t="s">
         <v>101</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D67" t="s">
         <v>329</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E67" t="s">
         <v>154</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F67" t="s">
         <v>356</v>
       </c>
-      <c r="G41" t="s">
+      <c r="G67" t="s">
         <v>132</v>
       </c>
-      <c r="H41" t="s">
+      <c r="H67" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>451</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B68" t="s">
         <v>452</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C68" t="s">
         <v>101</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D68" t="s">
         <v>338</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E68" t="s">
         <v>101</v>
       </c>
-      <c r="F42" t="s">
+      <c r="F68" t="s">
         <v>339</v>
       </c>
-      <c r="G42" t="s">
+      <c r="G68" t="s">
         <v>103</v>
       </c>
-      <c r="H42" t="s">
+      <c r="H68" t="s">
         <v>345</v>
       </c>
-      <c r="I42" t="s">
+      <c r="I68" t="s">
         <v>154</v>
       </c>
-      <c r="J42" t="s">
+      <c r="J68" t="s">
         <v>359</v>
       </c>
-      <c r="K42" t="s">
+      <c r="K68" t="s">
         <v>190</v>
       </c>
-      <c r="L42" t="s">
+      <c r="L68" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>453</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B69" t="s">
         <v>454</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C69" t="s">
         <v>204</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D69" t="s">
         <v>346</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E69" t="s">
         <v>101</v>
       </c>
-      <c r="F43" t="s">
+      <c r="F69" t="s">
         <v>434</v>
       </c>
-      <c r="G43" t="s">
+      <c r="G69" t="s">
         <v>143</v>
       </c>
-      <c r="H43" t="s">
+      <c r="H69" t="s">
         <v>455</v>
       </c>
-      <c r="I43" t="s">
+      <c r="I69" t="s">
         <v>123</v>
       </c>
-      <c r="J43" t="s">
+      <c r="J69" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>457</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B70" t="s">
         <v>458</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C70" t="s">
         <v>148</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D70" t="s">
         <v>455</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E70" t="s">
         <v>142</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F70" t="s">
         <v>459</v>
       </c>
-      <c r="G44" t="s">
+      <c r="G70" t="s">
         <v>161</v>
       </c>
-      <c r="H44" t="s">
+      <c r="H70" t="s">
         <v>322</v>
       </c>
-      <c r="I44" t="s">
+      <c r="I70" t="s">
         <v>189</v>
       </c>
-      <c r="J44" t="s">
+      <c r="J70" t="s">
         <v>374</v>
       </c>
-      <c r="K44" t="s">
+      <c r="K70" t="s">
         <v>190</v>
       </c>
-      <c r="L44" t="s">
+      <c r="L70" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>460</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B71" t="s">
         <v>461</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C71" t="s">
         <v>142</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D71" t="s">
         <v>455</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E71" t="s">
         <v>148</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F71" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>462</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B72" t="s">
         <v>463</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C72" t="s">
         <v>175</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D72" t="s">
         <v>464</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E72" t="s">
         <v>148</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F72" t="s">
         <v>375</v>
       </c>
-      <c r="G46" t="s">
+      <c r="G72" t="s">
         <v>151</v>
       </c>
-      <c r="H46" t="s">
+      <c r="H72" t="s">
         <v>323</v>
       </c>
-      <c r="I46" t="s">
+      <c r="I72" t="s">
         <v>190</v>
       </c>
-      <c r="J46" t="s">
+      <c r="J72" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>465</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B73" t="s">
         <v>466</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C73" t="s">
         <v>195</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D73" t="s">
         <v>467</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E73" t="s">
         <v>148</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F73" t="s">
         <v>468</v>
       </c>
-      <c r="G47" t="s">
+      <c r="G73" t="s">
         <v>142</v>
       </c>
-      <c r="H47" t="s">
+      <c r="H73" t="s">
         <v>311</v>
       </c>
-      <c r="I47" t="s">
+      <c r="I73" t="s">
         <v>190</v>
       </c>
-      <c r="J47" t="s">
+      <c r="J73" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>469</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B74" t="s">
         <v>300</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C74" t="s">
         <v>204</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D74" t="s">
         <v>470</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E74" t="s">
         <v>103</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F74" t="s">
         <v>430</v>
       </c>
-      <c r="G48" t="s">
+      <c r="G74" t="s">
         <v>143</v>
       </c>
-      <c r="H48" t="s">
+      <c r="H74" t="s">
         <v>317</v>
       </c>
-      <c r="I48" t="s">
+      <c r="I74" t="s">
         <v>152</v>
       </c>
-      <c r="J48" t="s">
+      <c r="J74" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>471</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B75" t="s">
         <v>472</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C75" t="s">
         <v>201</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D75" t="s">
         <v>473</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E75" t="s">
         <v>201</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F75" t="s">
         <v>329</v>
       </c>
-      <c r="G49" t="s">
+      <c r="G75" t="s">
         <v>474</v>
       </c>
-      <c r="H49" t="s">
+      <c r="H75" t="s">
         <v>329</v>
       </c>
-      <c r="I49" t="s">
+      <c r="I75" t="s">
         <v>151</v>
       </c>
-      <c r="J49" t="s">
+      <c r="J75" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>475</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B76" t="s">
         <v>476</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C76" t="s">
         <v>195</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D76" t="s">
         <v>477</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E76" t="s">
         <v>112</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F76" t="s">
         <v>374</v>
       </c>
-      <c r="G50" t="s">
+      <c r="G76" t="s">
         <v>117</v>
       </c>
-      <c r="H50" t="s">
+      <c r="H76" t="s">
         <v>478</v>
       </c>
-      <c r="I50" t="s">
+      <c r="I76" t="s">
         <v>97</v>
       </c>
-      <c r="J50" t="s">
+      <c r="J76" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>480</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B77" t="s">
         <v>297</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C77" t="s">
         <v>204</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D77" t="s">
         <v>375</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E77" t="s">
         <v>108</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F77" t="s">
         <v>367</v>
       </c>
-      <c r="G51" t="s">
+      <c r="G77" t="s">
         <v>134</v>
       </c>
-      <c r="H51" t="s">
+      <c r="H77" t="s">
         <v>367</v>
       </c>
-      <c r="I51" t="s">
+      <c r="I77" t="s">
         <v>184</v>
       </c>
-      <c r="J51" t="s">
+      <c r="J77" t="s">
         <v>322</v>
       </c>
-      <c r="K51" t="s">
+      <c r="K77" t="s">
         <v>146</v>
       </c>
-      <c r="L51" t="s">
+      <c r="L77" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>481</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B78" t="s">
         <v>298</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C78" t="s">
         <v>204</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D78" t="s">
         <v>375</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E78" t="s">
         <v>109</v>
       </c>
-      <c r="F52" t="s">
+      <c r="F78" t="s">
         <v>322</v>
       </c>
-      <c r="G52" t="s">
+      <c r="G78" t="s">
         <v>110</v>
       </c>
-      <c r="H52" t="s">
+      <c r="H78" t="s">
         <v>322</v>
       </c>
-      <c r="I52" t="s">
+      <c r="I78" t="s">
         <v>111</v>
       </c>
-      <c r="J52" t="s">
+      <c r="J78" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>482</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B79" t="s">
         <v>299</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C79" t="s">
         <v>204</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D79" t="s">
         <v>417</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E79" t="s">
         <v>103</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F79" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>858</v>
-      </c>
-      <c r="B54" t="s">
-        <v>859</v>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>915</v>
+      </c>
+      <c r="B80" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>917</v>
+      </c>
+      <c r="B81" t="s">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>918</v>
+      </c>
+      <c r="B82" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>920</v>
+      </c>
+      <c r="B83" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>921</v>
+      </c>
+      <c r="B84" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>922</v>
+      </c>
+      <c r="B85" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>923</v>
+      </c>
+      <c r="B86" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>924</v>
+      </c>
+      <c r="B87" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>925</v>
+      </c>
+      <c r="B88" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>926</v>
+      </c>
+      <c r="B89" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>931</v>
+      </c>
+      <c r="B90" t="s">
+        <v>919</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:V1" xr:uid="{93BD6150-B184-4D6F-9423-14648E8D4264}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:V79">
+      <sortCondition ref="B1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -8929,8 +9394,8 @@
   </sheetPr>
   <dimension ref="A1:C117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="H86" sqref="H86"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>